<commit_message>
Test plan implemented into Design Doc
</commit_message>
<xml_diff>
--- a/MAD3TestPlan.xlsx
+++ b/MAD3TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G00338607\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G00338607\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221CF18B-4B7E-4B63-BDD5-53BF98558E2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3356335D-B689-4EA4-A617-C5AAB858FF85}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="225" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monkey March" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="159">
   <si>
     <t>Purpose:</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Actual Result</t>
   </si>
   <si>
-    <t>Successful login</t>
-  </si>
-  <si>
     <t>Test Case Name</t>
   </si>
   <si>
@@ -93,22 +90,12 @@
     <t>TC.008</t>
   </si>
   <si>
-    <t>Successful login to application</t>
-  </si>
-  <si>
     <t>TC.009</t>
   </si>
   <si>
-    <t>Unsuccessful login to application
-Message displayed "Wrong password used, please recheck"</t>
-  </si>
-  <si>
     <t>TC.010</t>
   </si>
   <si>
-    <t>Details of new login credentals emailed to client</t>
-  </si>
-  <si>
     <t>TC.011</t>
   </si>
   <si>
@@ -118,35 +105,16 @@
     <t>TC.013</t>
   </si>
   <si>
-    <t>Email notifications received in Gmail and Outlook</t>
-  </si>
-  <si>
     <t>TC.014</t>
   </si>
   <si>
     <t>TC.015</t>
   </si>
   <si>
-    <t>Successful login using Facebook credentials</t>
-  </si>
-  <si>
     <t>TC.017</t>
   </si>
   <si>
-    <t>Successful login using 
-Google+ credentials</t>
-  </si>
-  <si>
     <t>TC.016</t>
-  </si>
-  <si>
-    <t>Unsuccessful login</t>
-  </si>
-  <si>
-    <t>New login details emailed to client</t>
-  </si>
-  <si>
-    <t>Email notifications received for login details</t>
   </si>
   <si>
     <t>Monkey March</t>
@@ -310,27 +278,7 @@
 3. Select Difficulty                               4. Start Game                                      5. Get hit by rocks or fall into pit    6. Health decreases</t>
   </si>
   <si>
-    <t>1. Launch Game
-2.  Select New Game
-3. Select Difficulty                               4. Start Game                                      5. Finish Game or at least die       6. Score appears</t>
-  </si>
-  <si>
     <t>Game Ending</t>
-  </si>
-  <si>
-    <t>1. Launch Game
-2.  Select New Game
-3. Select Difficulty                               4. Start Game                                      5. Finish Game or at least die       6. Score appears                                 7. Select to Play Again</t>
-  </si>
-  <si>
-    <t>1. Launch Game
-2.  Select New Game
-3. Select Difficulty                               4. Start Game                                      5. Finish Game or at least die       6. Score appears                                 7. Select to Exit to main menu</t>
-  </si>
-  <si>
-    <t>1. Launch Game
-2.  Select New Game
-3. Select Difficulty                               4. Start Game                                      5. Finish Game or at least die       6. Score appears                                 7. Select settings</t>
   </si>
   <si>
     <t>TC.018</t>
@@ -487,13 +435,123 @@
   </si>
   <si>
     <t>Touch appear</t>
+  </si>
+  <si>
+    <t>Checks if user can pause the game in middle of a session</t>
+  </si>
+  <si>
+    <t>Checks if the user can change various settings such as Audio and Control preferences</t>
+  </si>
+  <si>
+    <t>Audio is muted or un-muted and control preferences change</t>
+  </si>
+  <si>
+    <t>Audio is muted and control prefernces change to touch</t>
+  </si>
+  <si>
+    <t>Game is paused</t>
+  </si>
+  <si>
+    <t>Game pauses</t>
+  </si>
+  <si>
+    <t>Checks if user can continue the game they just paused by selecting Continue</t>
+  </si>
+  <si>
+    <t>Game should continue</t>
+  </si>
+  <si>
+    <t>Game continues</t>
+  </si>
+  <si>
+    <t>Checks if user can save the game they just paused by selecting Save Game</t>
+  </si>
+  <si>
+    <t>Game should save</t>
+  </si>
+  <si>
+    <t>User should exit to main menu</t>
+  </si>
+  <si>
+    <t>Game saves</t>
+  </si>
+  <si>
+    <t>User exits to main menu</t>
+  </si>
+  <si>
+    <t>Checks if user can exit the game they just paused, and will end up at the main menu</t>
+  </si>
+  <si>
+    <t>Checks if user Health&amp;Score increases via collecting tokens</t>
+  </si>
+  <si>
+    <t>Checks if user Health decreases</t>
+  </si>
+  <si>
+    <t>Health decreases by 20%</t>
+  </si>
+  <si>
+    <t>Health increases by 10% and Score increases by 2</t>
+  </si>
+  <si>
+    <t>Health should increase by 10% and Score should increase by 1</t>
+  </si>
+  <si>
+    <t>Health should decrease by 20%</t>
+  </si>
+  <si>
+    <t>1. Launch Game
+2.  Select New Game
+3. Select Difficulty                               4. Start Game                                      5. Finish Game or at least die           6. Score appears</t>
+  </si>
+  <si>
+    <t>Checks if a score appears when the user dies or completes a level</t>
+  </si>
+  <si>
+    <t>Score should appear</t>
+  </si>
+  <si>
+    <t>Score appears</t>
+  </si>
+  <si>
+    <t>1. Launch Game
+2.  Select New Game
+3. Select Difficulty                               4. Start Game                                      5. Finish Game or at least die           6. Score appears                                 7. Select to Play Again</t>
+  </si>
+  <si>
+    <t>1. Launch Game
+2.  Select New Game
+3. Select Difficulty                               4. Start Game                                      5. Finish Game or at least die           6. Score appears                                 7. Select to Exit to main menu</t>
+  </si>
+  <si>
+    <t>1. Launch Game
+2.  Select New Game
+3. Select Difficulty                               4. Start Game                                      5. Finish Game or at least die           6. Score appears                                 7. Select settings</t>
+  </si>
+  <si>
+    <t>Checks if user is able to play again once game has ended</t>
+  </si>
+  <si>
+    <t>New game session should load in</t>
+  </si>
+  <si>
+    <t>New game session has started</t>
+  </si>
+  <si>
+    <t>Checks if user can exit to the main menu once the game has enced and a score has appeared</t>
+  </si>
+  <si>
+    <t>Checks if user can change settings even when a game has ended</t>
+  </si>
+  <si>
+    <t>Settings menu should appear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,13 +580,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15.4"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Verdana"/>
@@ -537,6 +588,20 @@
     <font>
       <b/>
       <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -708,10 +773,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -732,22 +797,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1154,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,10 +1245,10 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="19"/>
+      <c r="D1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="16"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -1194,12 +1259,12 @@
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="20"/>
+        <v>33</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="17"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="2"/>
@@ -1209,16 +1274,16 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" s="6" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="17"/>
+      <c r="A3" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="20"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1237,7 +1302,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>2</v>
@@ -1275,22 +1340,22 @@
         <v>10</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>108</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>11</v>
@@ -1309,22 +1374,22 @@
         <v>12</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>11</v>
@@ -1343,22 +1408,22 @@
         <v>13</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="G7" s="9" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>11</v>
@@ -1368,31 +1433,31 @@
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B8" s="10">
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>11</v>
@@ -1402,31 +1467,31 @@
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B9" s="10">
         <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>11</v>
@@ -1442,25 +1507,25 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>11</v>
@@ -1476,25 +1541,25 @@
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>11</v>
@@ -1504,31 +1569,31 @@
     </row>
     <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B12" s="10">
         <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>11</v>
@@ -1538,31 +1603,31 @@
     </row>
     <row r="13" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B13" s="10">
         <v>1</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="J13" s="10" t="s">
         <v>11</v>
@@ -1572,31 +1637,31 @@
     </row>
     <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B14" s="10">
         <v>1</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="J14" s="10" t="s">
         <v>11</v>
@@ -1606,31 +1671,31 @@
     </row>
     <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B15" s="10">
         <v>1</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="J15" s="10" t="s">
         <v>11</v>
@@ -1640,31 +1705,31 @@
     </row>
     <row r="16" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B16" s="10">
         <v>1</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="J16" s="10" t="s">
         <v>11</v>
@@ -1674,31 +1739,31 @@
     </row>
     <row r="17" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B17" s="10">
         <v>1</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>65</v>
-      </c>
       <c r="G17" s="9" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="J17" s="10" t="s">
         <v>11</v>
@@ -1708,31 +1773,31 @@
     </row>
     <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B18" s="10">
         <v>1</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="J18" s="10" t="s">
         <v>11</v>
@@ -1748,25 +1813,25 @@
         <v>1</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="J19" s="10" t="s">
         <v>11</v>
@@ -1774,7 +1839,7 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
     </row>
-    <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>3.1</v>
       </c>
@@ -1782,25 +1847,25 @@
         <v>1</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="J20" s="10" t="s">
         <v>11</v>
@@ -1810,31 +1875,31 @@
     </row>
     <row r="21" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B21" s="10">
         <v>1</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="J21" s="10" t="s">
         <v>11</v>
@@ -1844,31 +1909,31 @@
     </row>
     <row r="22" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="10">
-        <v>1</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>88</v>
-      </c>
       <c r="D22" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>36</v>
+        <v>135</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="J22" s="10" t="s">
         <v>11</v>
@@ -1878,31 +1943,31 @@
     </row>
     <row r="23" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="10">
-        <v>1</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="D23" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="J23" s="10" t="s">
         <v>11</v>
@@ -1918,25 +1983,25 @@
         <v>1</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>16</v>
+        <v>143</v>
       </c>
       <c r="J24" s="10" t="s">
         <v>11</v>
@@ -1944,7 +2009,7 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
     </row>
-    <row r="25" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>4.2</v>
       </c>
@@ -1952,25 +2017,25 @@
         <v>1</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>38</v>
+        <v>142</v>
       </c>
       <c r="J25" s="10" t="s">
         <v>11</v>
@@ -1986,25 +2051,25 @@
         <v>1</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>27</v>
+        <v>148</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>39</v>
+        <v>149</v>
       </c>
       <c r="J26" s="10" t="s">
         <v>11</v>
@@ -2020,25 +2085,25 @@
         <v>1</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>31</v>
+        <v>154</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="J27" s="10" t="s">
         <v>11</v>
@@ -2054,25 +2119,25 @@
         <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>94</v>
+        <v>156</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>40</v>
+        <v>138</v>
       </c>
       <c r="J28" s="10" t="s">
         <v>11</v>
@@ -2082,31 +2147,31 @@
     </row>
     <row r="29" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B29" s="10">
         <v>1</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>34</v>
+        <v>158</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="J29" s="10" t="s">
         <v>11</v>

</xml_diff>